<commit_message>
Updated task event dates and supervisor workflows
</commit_message>
<xml_diff>
--- a/cht_oppia_mvp/forms/app/cha_module_three.xlsx
+++ b/cht_oppia_mvp/forms/app/cha_module_three.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="152">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -185,8 +185,30 @@
     <t xml:space="preserve">learning_quiz</t>
   </si>
   <si>
-    <t xml:space="preserve">Assessment
-We would like to ask you a few questions to understand your knowledge on COVID-19 in regards to this module:</t>
+    <t xml:space="preserve">Assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessment_note</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.4"/>
+        <color rgb="FF4C4C4C"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">We would like to ask you a few questions to understand your knowledge on COVID-19 in regards to this module:**</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">select_one true_false</t>
@@ -207,7 +229,7 @@
     <t xml:space="preserve">NO_LABEL</t>
   </si>
   <si>
-    <t xml:space="preserve">if(selected(${who_attacked_q},’true’), 1, 0)</t>
+    <t xml:space="preserve">if(selected(${who_attacked_q},’false’), 1, 0)</t>
   </si>
   <si>
     <t xml:space="preserve">no_covid_vaccine_q</t>
@@ -222,22 +244,16 @@
     <t xml:space="preserve">if(selected(${no_covid_vaccine_q},’true’), 1, 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">select_multiple true_false</t>
-  </si>
-  <si>
     <t xml:space="preserve">like_malaria_q</t>
   </si>
   <si>
     <t xml:space="preserve">3. COVID is like Malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Select all that apply</t>
-  </si>
-  <si>
     <t xml:space="preserve">like_malaria_score</t>
   </si>
   <si>
-    <t xml:space="preserve">if(selected(${like_malaria_q},’true’), 1, 0)</t>
+    <t xml:space="preserve">if(selected(${like_malaria_q},’false’), 1, 0)</t>
   </si>
   <si>
     <t xml:space="preserve">strong_disinfectant_q</t>
@@ -249,7 +265,7 @@
     <t xml:space="preserve">strong_disinfectant_score</t>
   </si>
   <si>
-    <t xml:space="preserve">if(selected(${strong_disinfectant_q},’true’), 1, 0)</t>
+    <t xml:space="preserve">if(selected(${strong_disinfectant_q},’false’), 1, 0)</t>
   </si>
   <si>
     <t xml:space="preserve">select_multiple fight_misinformation</t>
@@ -303,59 +319,59 @@
     <t xml:space="preserve">thank_you_note</t>
   </si>
   <si>
-    <t xml:space="preserve">Good start, but you only answered **scored ${assessment_score}** out of the 8 questions correctly.
+    <t xml:space="preserve">Good start, but you only answered **scored ${assessment_score}** out of the **5** questions correctly.
 This task will not be completed until you answer all the questions correctly</t>
   </si>
   <si>
     <t xml:space="preserve">${assessment_passed} = ‘no’</t>
   </si>
   <si>
+    <t xml:space="preserve">Do you need additional support on this topic?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">success_note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great job! You have completed Module 3: Misinformation. You can revisit this content at any time in your Oppia app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${assessment_passed} = ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confidence_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**The following questions are designed to understand your confidence to perform the tasks taught in this lesson.**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gauge_mastery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Following this training, what is your level of confidence that you can effectively perform the following tasks related to COVID-19?**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one confidence_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transmission_confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Address rumours on COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preventive_measures_confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Recognize and address misinformation on COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have any other questions or feedback on this topic?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you need additional support on this topic?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">success_note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great job! You have completed Module 3: Misinformation. You can revisit this content at any time in your Oppia app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${assessment_passed} = ‘yes’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confidence_level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**The following questions are designed to understand your confidence to perform the tasks taught in this lesson.**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gauge_mastery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Following this training, what is your level of confidence that you can effectively perform the following tasks related to COVID-19?**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one confidence_level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transmission_confidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Address rumours on COVID-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preventive_measures_confidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Recognize and address misinformation on COVID-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feedback</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have any other questions or feedback on this topic?</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -493,7 +509,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -535,6 +551,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -668,7 +690,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,15 +698,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,7 +714,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -773,14 +795,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB46"/>
+  <dimension ref="A1:BB47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1089,7 +1111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" s="4" customFormat="true" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -1103,205 +1125,202 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="21" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="J23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>35</v>
+      <c r="A24" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="8" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L25" s="1" t="s">
+      <c r="C26" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="C31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
+    <row r="32" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+    <row r="35" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="4" t="s">
+      <c r="C35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1309,164 +1328,172 @@
         <v>43</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="C38" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="1" t="s">
+    </row>
+    <row r="41" s="10" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" s="10" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
+      <c r="C41" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="11" t="s">
+      <c r="B42" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C42" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="D44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
+    <row r="47" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1519,7 +1546,7 @@
         <v>114</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>115</v>
@@ -1538,7 +1565,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>118</v>
@@ -1549,7 +1576,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>120</v>
@@ -1560,7 +1587,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>122</v>
@@ -1571,7 +1598,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>124</v>
@@ -1582,7 +1609,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>126</v>
@@ -1717,7 +1744,7 @@
       </c>
       <c r="C2" s="15" t="n">
         <f aca="true">NOW()</f>
-        <v>44091.761874274</v>
+        <v>44105.6246081268</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>150</v>

</xml_diff>